<commit_message>
Test-1 for hybrid model (MAPE)
</commit_message>
<xml_diff>
--- a/migforecasting/Hybridization/exp/test 1.xlsx
+++ b/migforecasting/Hybridization/exp/test 1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="11">
   <si>
     <t>test size 20%</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>test (MAPE)</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -99,13 +105,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:U59"/>
+  <dimension ref="D4:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,9 +413,13 @@
     <col min="16" max="16" width="14.28515625" customWidth="1"/>
     <col min="20" max="20" width="13.85546875" customWidth="1"/>
     <col min="21" max="21" width="14.5703125" customWidth="1"/>
+    <col min="25" max="25" width="11.85546875" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" customWidth="1"/>
+    <col min="32" max="32" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="4:32" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,8 +432,14 @@
       <c r="T4" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="Y4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>1</v>
       </c>
@@ -437,8 +456,16 @@
         <v>6</v>
       </c>
       <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="X5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1"/>
+      <c r="AD5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>2</v>
@@ -467,8 +494,22 @@
       <c r="U6" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D7" s="2">
         <v>1</v>
       </c>
@@ -499,10 +540,28 @@
       <c r="S7" s="2">
         <v>1</v>
       </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T7" s="3">
+        <v>1.109086872599091</v>
+      </c>
+      <c r="U7" s="3">
+        <v>2.559622646169089</v>
+      </c>
+      <c r="X7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>8.7310959796989903E-4</v>
+      </c>
+      <c r="Z7" s="4">
+        <v>5.932368422197627E-3</v>
+      </c>
+      <c r="AD7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="4"/>
+      <c r="AF7" s="4"/>
+    </row>
+    <row r="8" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
         <f>D7+1</f>
         <v>2</v>
@@ -537,10 +596,30 @@
         <f>S7+1</f>
         <v>2</v>
       </c>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-    </row>
-    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T8" s="3">
+        <v>1.2942635099514119</v>
+      </c>
+      <c r="U8" s="3">
+        <v>2.4828945934840161</v>
+      </c>
+      <c r="X8" s="2">
+        <f>X7+1</f>
+        <v>2</v>
+      </c>
+      <c r="Y8" s="4">
+        <v>8.7054759684879939E-4</v>
+      </c>
+      <c r="Z8" s="4">
+        <v>5.8219286043002458E-3</v>
+      </c>
+      <c r="AD8" s="2">
+        <f>AD7+1</f>
+        <v>2</v>
+      </c>
+      <c r="AE8" s="4"/>
+      <c r="AF8" s="4"/>
+    </row>
+    <row r="9" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
         <f t="shared" ref="D9:D56" si="0">D8+1</f>
         <v>3</v>
@@ -575,10 +654,30 @@
         <f t="shared" ref="S9:S56" si="3">S8+1</f>
         <v>3</v>
       </c>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-    </row>
-    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T9" s="3">
+        <v>1.262206838219325</v>
+      </c>
+      <c r="U9" s="3">
+        <v>1.8707805243102751</v>
+      </c>
+      <c r="X9" s="2">
+        <f t="shared" ref="X9:X56" si="4">X8+1</f>
+        <v>3</v>
+      </c>
+      <c r="Y9" s="4">
+        <v>8.9078371730447724E-4</v>
+      </c>
+      <c r="Z9" s="4">
+        <v>5.3389520975033553E-3</v>
+      </c>
+      <c r="AD9" s="2">
+        <f t="shared" ref="AD9:AD56" si="5">AD8+1</f>
+        <v>3</v>
+      </c>
+      <c r="AE9" s="4"/>
+      <c r="AF9" s="4"/>
+    </row>
+    <row r="10" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -613,10 +712,30 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-    </row>
-    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T10" s="3">
+        <v>1.3717592324603289</v>
+      </c>
+      <c r="U10" s="3">
+        <v>1.5207616143197009</v>
+      </c>
+      <c r="X10" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="Y10" s="4">
+        <v>9.2412889899268051E-4</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>5.9228166490137221E-3</v>
+      </c>
+      <c r="AD10" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AE10" s="4"/>
+      <c r="AF10" s="4"/>
+    </row>
+    <row r="11" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -651,10 +770,30 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-    </row>
-    <row r="12" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T11" s="3">
+        <v>0.75086986220693375</v>
+      </c>
+      <c r="U11" s="3">
+        <v>6.6283542790069383</v>
+      </c>
+      <c r="X11" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>9.7348016341827228E-4</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>4.8803194488362374E-3</v>
+      </c>
+      <c r="AD11" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4"/>
+    </row>
+    <row r="12" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -689,10 +828,30 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T12" s="3">
+        <v>0.99350411581429832</v>
+      </c>
+      <c r="U12" s="3">
+        <v>1.6808313241741839</v>
+      </c>
+      <c r="X12" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Y12" s="4">
+        <v>9.0423577436433067E-4</v>
+      </c>
+      <c r="Z12" s="4">
+        <v>6.452537677104647E-3</v>
+      </c>
+      <c r="AD12" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AE12" s="4"/>
+      <c r="AF12" s="4"/>
+    </row>
+    <row r="13" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -727,10 +886,30 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T13" s="3">
+        <v>1.078750600763283</v>
+      </c>
+      <c r="U13" s="3">
+        <v>3.4126613846272229</v>
+      </c>
+      <c r="X13" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Y13" s="4">
+        <v>8.4642562284647995E-4</v>
+      </c>
+      <c r="Z13" s="4">
+        <v>6.5450990290021006E-3</v>
+      </c>
+      <c r="AD13" s="2">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AE13" s="4"/>
+      <c r="AF13" s="4"/>
+    </row>
+    <row r="14" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -765,10 +944,30 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T14" s="3">
+        <v>1.241482451169164</v>
+      </c>
+      <c r="U14" s="3">
+        <v>2.3127844288398141</v>
+      </c>
+      <c r="X14" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="Y14" s="4">
+        <v>8.6699652935646305E-4</v>
+      </c>
+      <c r="Z14" s="4">
+        <v>7.081593320648184E-3</v>
+      </c>
+      <c r="AD14" s="2">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4"/>
+    </row>
+    <row r="15" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -803,10 +1002,30 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T15" s="3">
+        <v>1.088308306751306</v>
+      </c>
+      <c r="U15" s="3">
+        <v>2.5418018019155841</v>
+      </c>
+      <c r="X15" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>8.9935724886711869E-4</v>
+      </c>
+      <c r="Z15" s="4">
+        <v>6.712956779829425E-3</v>
+      </c>
+      <c r="AD15" s="2">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AE15" s="4"/>
+      <c r="AF15" s="4"/>
+    </row>
+    <row r="16" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -841,10 +1060,30 @@
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T16" s="3">
+        <v>1.136015189224052</v>
+      </c>
+      <c r="U16" s="3">
+        <v>2.7378819525664788</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>9.2270630303479411E-4</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>4.3575756158191082E-3</v>
+      </c>
+      <c r="AD16" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AE16" s="4"/>
+      <c r="AF16" s="4"/>
+    </row>
+    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -879,10 +1118,30 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
-    </row>
-    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T17" s="3">
+        <v>1.212628168714994</v>
+      </c>
+      <c r="U17" s="3">
+        <v>3.5327611285644971</v>
+      </c>
+      <c r="X17" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>7.9329877704101184E-4</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>7.5987457294741916E-3</v>
+      </c>
+      <c r="AD17" s="2">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AE17" s="4"/>
+      <c r="AF17" s="4"/>
+    </row>
+    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -917,10 +1176,30 @@
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T18" s="3">
+        <v>1.287743677463741</v>
+      </c>
+      <c r="U18" s="3">
+        <v>1.340048169013204</v>
+      </c>
+      <c r="X18" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>8.6272176049172742E-4</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>5.3502305808586607E-3</v>
+      </c>
+      <c r="AD18" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+    </row>
+    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -955,10 +1234,30 @@
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T19" s="3">
+        <v>1.089018964567724</v>
+      </c>
+      <c r="U19" s="3">
+        <v>2.0567579677097521</v>
+      </c>
+      <c r="X19" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>9.2209056998013446E-4</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>6.664244090777649E-3</v>
+      </c>
+      <c r="AD19" s="2">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AE19" s="4"/>
+      <c r="AF19" s="4"/>
+    </row>
+    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -993,10 +1292,30 @@
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
-    </row>
-    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T20" s="3">
+        <v>1.0519333675869791</v>
+      </c>
+      <c r="U20" s="3">
+        <v>4.7894325023372044</v>
+      </c>
+      <c r="X20" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="Y20" s="4">
+        <v>7.6493865361732644E-4</v>
+      </c>
+      <c r="Z20" s="4">
+        <v>9.1663036030846818E-3</v>
+      </c>
+      <c r="AD20" s="2">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="AE20" s="4"/>
+      <c r="AF20" s="4"/>
+    </row>
+    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1031,10 +1350,30 @@
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="T21" s="3"/>
-      <c r="U21" s="3"/>
-    </row>
-    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T21" s="3">
+        <v>1.002878055679282</v>
+      </c>
+      <c r="U21" s="3">
+        <v>4.9373573140135312</v>
+      </c>
+      <c r="X21" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Y21" s="4">
+        <v>8.5648234863549579E-4</v>
+      </c>
+      <c r="Z21" s="4">
+        <v>7.8483034925778804E-3</v>
+      </c>
+      <c r="AD21" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="4"/>
+    </row>
+    <row r="22" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1069,10 +1408,30 @@
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
-    </row>
-    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T22" s="3">
+        <v>0.99939054779466707</v>
+      </c>
+      <c r="U22" s="3">
+        <v>1.740158778914588</v>
+      </c>
+      <c r="X22" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="Y22" s="4">
+        <v>8.9941608027565895E-4</v>
+      </c>
+      <c r="Z22" s="4">
+        <v>5.8490371152067188E-3</v>
+      </c>
+      <c r="AD22" s="2">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="4"/>
+    </row>
+    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1107,10 +1466,30 @@
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
-    </row>
-    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T23" s="3">
+        <v>0.95097117822238986</v>
+      </c>
+      <c r="U23" s="3">
+        <v>4.1622779894104873</v>
+      </c>
+      <c r="X23" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Y23" s="4">
+        <v>9.6831375624059732E-4</v>
+      </c>
+      <c r="Z23" s="4">
+        <v>4.9253349369959383E-3</v>
+      </c>
+      <c r="AD23" s="2">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AE23" s="4"/>
+      <c r="AF23" s="4"/>
+    </row>
+    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1145,10 +1524,30 @@
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
-    </row>
-    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T24" s="3">
+        <v>0.8147904789812721</v>
+      </c>
+      <c r="U24" s="3">
+        <v>4.7416597215325957</v>
+      </c>
+      <c r="X24" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="Y24" s="4">
+        <v>7.8706374006531313E-4</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>7.0166700063517707E-3</v>
+      </c>
+      <c r="AD24" s="2">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AE24" s="4"/>
+      <c r="AF24" s="4"/>
+    </row>
+    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1183,10 +1582,30 @@
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-    </row>
-    <row r="26" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T25" s="3">
+        <v>0.79633151004290126</v>
+      </c>
+      <c r="U25" s="3">
+        <v>5.5607081944653052</v>
+      </c>
+      <c r="X25" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="Y25" s="4">
+        <v>9.262975969762064E-4</v>
+      </c>
+      <c r="Z25" s="4">
+        <v>5.2188839667433066E-3</v>
+      </c>
+      <c r="AD25" s="2">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AE25" s="4"/>
+      <c r="AF25" s="4"/>
+    </row>
+    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1221,10 +1640,30 @@
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T26" s="3">
+        <v>1.0931469136063341</v>
+      </c>
+      <c r="U26" s="3">
+        <v>4.9880012804616847</v>
+      </c>
+      <c r="X26" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="Y26" s="4">
+        <v>9.4145891132320825E-4</v>
+      </c>
+      <c r="Z26" s="4">
+        <v>5.1420285299677527E-3</v>
+      </c>
+      <c r="AD26" s="2">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AE26" s="4"/>
+      <c r="AF26" s="4"/>
+    </row>
+    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1259,10 +1698,30 @@
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T27" s="3">
+        <v>1.06901132716129</v>
+      </c>
+      <c r="U27" s="3">
+        <v>2.0125013282259112</v>
+      </c>
+      <c r="X27" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="Y27" s="4">
+        <v>8.7841927228379997E-4</v>
+      </c>
+      <c r="Z27" s="4">
+        <v>4.9091243264284606E-3</v>
+      </c>
+      <c r="AD27" s="2">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
+    </row>
+    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1297,10 +1756,30 @@
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
-    </row>
-    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T28" s="3">
+        <v>1.035610076811184</v>
+      </c>
+      <c r="U28" s="3">
+        <v>2.3303592876257571</v>
+      </c>
+      <c r="X28" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="Y28" s="4">
+        <v>8.4295102475085858E-4</v>
+      </c>
+      <c r="Z28" s="4">
+        <v>6.1897513399513026E-3</v>
+      </c>
+      <c r="AD28" s="2">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AE28" s="4"/>
+      <c r="AF28" s="4"/>
+    </row>
+    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1335,10 +1814,30 @@
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
-    </row>
-    <row r="30" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T29" s="3">
+        <v>1.2812004230259131</v>
+      </c>
+      <c r="U29" s="3">
+        <v>2.329148958704371</v>
+      </c>
+      <c r="X29" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="Y29" s="4">
+        <v>8.9120654656589299E-4</v>
+      </c>
+      <c r="Z29" s="4">
+        <v>5.2295782136074376E-3</v>
+      </c>
+      <c r="AD29" s="2">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+    </row>
+    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1373,10 +1872,30 @@
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-    </row>
-    <row r="31" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T30" s="3">
+        <v>0.95532358523180716</v>
+      </c>
+      <c r="U30" s="3">
+        <v>4.8846415477137448</v>
+      </c>
+      <c r="X30" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="Y30" s="4">
+        <v>9.8355924384296552E-4</v>
+      </c>
+      <c r="Z30" s="4">
+        <v>4.4088195443491886E-3</v>
+      </c>
+      <c r="AD30" s="2">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AE30" s="4"/>
+      <c r="AF30" s="4"/>
+    </row>
+    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1411,10 +1930,30 @@
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-    </row>
-    <row r="32" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T31" s="3">
+        <v>1.258127442532762</v>
+      </c>
+      <c r="U31" s="3">
+        <v>3.028164595782072</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="Y31" s="4">
+        <v>8.6127567909827739E-4</v>
+      </c>
+      <c r="Z31" s="4">
+        <v>6.8137955750758802E-3</v>
+      </c>
+      <c r="AD31" s="2">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AE31" s="4"/>
+      <c r="AF31" s="4"/>
+    </row>
+    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1449,10 +1988,30 @@
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
-    </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T32" s="3">
+        <v>1.0669812056973429</v>
+      </c>
+      <c r="U32" s="3">
+        <v>2.4778894259913282</v>
+      </c>
+      <c r="X32" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="Y32" s="4">
+        <v>8.5793298368885677E-4</v>
+      </c>
+      <c r="Z32" s="4">
+        <v>8.3836850514006026E-3</v>
+      </c>
+      <c r="AD32" s="2">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AE32" s="4"/>
+      <c r="AF32" s="4"/>
+    </row>
+    <row r="33" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1487,10 +2046,30 @@
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
-    </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T33" s="3">
+        <v>0.7829831974026279</v>
+      </c>
+      <c r="U33" s="3">
+        <v>5.4007467001098339</v>
+      </c>
+      <c r="X33" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="Y33" s="4">
+        <v>8.8296522610342048E-4</v>
+      </c>
+      <c r="Z33" s="4">
+        <v>6.254123444370035E-3</v>
+      </c>
+      <c r="AD33" s="2">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+    </row>
+    <row r="34" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1525,10 +2104,30 @@
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
-    </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T34" s="3">
+        <v>0.94911802246323396</v>
+      </c>
+      <c r="U34" s="3">
+        <v>4.1598487687875192</v>
+      </c>
+      <c r="X34" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="Y34" s="4">
+        <v>8.8189256340739702E-4</v>
+      </c>
+      <c r="Z34" s="4">
+        <v>4.8209854126703283E-3</v>
+      </c>
+      <c r="AD34" s="2">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+    </row>
+    <row r="35" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1563,10 +2162,30 @@
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
-    </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T35" s="3">
+        <v>0.8948692202300621</v>
+      </c>
+      <c r="U35" s="3">
+        <v>3.2056803332862209</v>
+      </c>
+      <c r="X35" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="Y35" s="4">
+        <v>9.1663038075533404E-4</v>
+      </c>
+      <c r="Z35" s="4">
+        <v>5.8413571107318787E-3</v>
+      </c>
+      <c r="AD35" s="2">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+    </row>
+    <row r="36" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1601,10 +2220,30 @@
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
-    </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T36" s="3">
+        <v>0.94362599071935849</v>
+      </c>
+      <c r="U36" s="3">
+        <v>5.0846920873446519</v>
+      </c>
+      <c r="X36" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="Y36" s="4">
+        <v>7.8899438645142642E-4</v>
+      </c>
+      <c r="Z36" s="4">
+        <v>9.4701684497667579E-3</v>
+      </c>
+      <c r="AD36" s="2">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+    </row>
+    <row r="37" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1639,10 +2278,30 @@
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
-      <c r="T37" s="3"/>
-      <c r="U37" s="3"/>
-    </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T37" s="3">
+        <v>1.1257450845651971</v>
+      </c>
+      <c r="U37" s="3">
+        <v>1.982311840776849</v>
+      </c>
+      <c r="X37" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Y37" s="4">
+        <v>8.6187439991011533E-4</v>
+      </c>
+      <c r="Z37" s="4">
+        <v>5.383488897508692E-3</v>
+      </c>
+      <c r="AD37" s="2">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+    </row>
+    <row r="38" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1677,10 +2336,30 @@
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="T38" s="3"/>
-      <c r="U38" s="3"/>
-    </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T38" s="3">
+        <v>1.1868648930436969</v>
+      </c>
+      <c r="U38" s="3">
+        <v>1.7441251130469979</v>
+      </c>
+      <c r="X38" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="Y38" s="4">
+        <v>8.1945664294456487E-4</v>
+      </c>
+      <c r="Z38" s="4">
+        <v>8.8199934821025817E-3</v>
+      </c>
+      <c r="AD38" s="2">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="AE38" s="4"/>
+      <c r="AF38" s="4"/>
+    </row>
+    <row r="39" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1715,10 +2394,30 @@
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
-    </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T39" s="3">
+        <v>1.284347951580713</v>
+      </c>
+      <c r="U39" s="3">
+        <v>1.9205793353055109</v>
+      </c>
+      <c r="X39" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="Y39" s="4">
+        <v>7.8407001413694649E-4</v>
+      </c>
+      <c r="Z39" s="4">
+        <v>7.9862340409000299E-3</v>
+      </c>
+      <c r="AD39" s="2">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4"/>
+    </row>
+    <row r="40" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1753,10 +2452,30 @@
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
-    </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T40" s="3">
+        <v>1.0263360381953399</v>
+      </c>
+      <c r="U40" s="3">
+        <v>3.3374948292533819</v>
+      </c>
+      <c r="X40" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="Y40" s="4">
+        <v>8.9696083082663148E-4</v>
+      </c>
+      <c r="Z40" s="4">
+        <v>5.5065293687982806E-3</v>
+      </c>
+      <c r="AD40" s="2">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="AE40" s="4"/>
+      <c r="AF40" s="4"/>
+    </row>
+    <row r="41" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1791,10 +2510,30 @@
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
-    </row>
-    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T41" s="3">
+        <v>0.9353764648925692</v>
+      </c>
+      <c r="U41" s="3">
+        <v>4.9721264644255667</v>
+      </c>
+      <c r="X41" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="Y41" s="4">
+        <v>9.1559517486767086E-4</v>
+      </c>
+      <c r="Z41" s="4">
+        <v>6.3514971919654212E-3</v>
+      </c>
+      <c r="AD41" s="2">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="AE41" s="4"/>
+      <c r="AF41" s="4"/>
+    </row>
+    <row r="42" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1829,10 +2568,30 @@
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-    </row>
-    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T42" s="3">
+        <v>1.074325318984271</v>
+      </c>
+      <c r="U42" s="3">
+        <v>1.656382032469949</v>
+      </c>
+      <c r="X42" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="Y42" s="4">
+        <v>8.8953667395526368E-4</v>
+      </c>
+      <c r="Z42" s="4">
+        <v>6.2632808780881226E-3</v>
+      </c>
+      <c r="AD42" s="2">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="AE42" s="4"/>
+      <c r="AF42" s="4"/>
+    </row>
+    <row r="43" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1867,10 +2626,30 @@
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-    </row>
-    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T43" s="3">
+        <v>1.1619194307686489</v>
+      </c>
+      <c r="U43" s="3">
+        <v>1.823686166107177</v>
+      </c>
+      <c r="X43" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="Y43" s="4">
+        <v>8.5012328763200181E-4</v>
+      </c>
+      <c r="Z43" s="4">
+        <v>7.5876136563189757E-3</v>
+      </c>
+      <c r="AD43" s="2">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="AE43" s="4"/>
+      <c r="AF43" s="4"/>
+    </row>
+    <row r="44" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1905,10 +2684,30 @@
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-    </row>
-    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T44" s="3">
+        <v>1.2349624752526851</v>
+      </c>
+      <c r="U44" s="3">
+        <v>1.721686843496484</v>
+      </c>
+      <c r="X44" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="Y44" s="4">
+        <v>8.2471618472576048E-4</v>
+      </c>
+      <c r="Z44" s="4">
+        <v>8.2139286633500612E-3</v>
+      </c>
+      <c r="AD44" s="2">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="AE44" s="4"/>
+      <c r="AF44" s="4"/>
+    </row>
+    <row r="45" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1943,10 +2742,30 @@
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-    </row>
-    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T45" s="3">
+        <v>1.2593474008940011</v>
+      </c>
+      <c r="U45" s="3">
+        <v>1.6380100206562229</v>
+      </c>
+      <c r="X45" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="Y45" s="4">
+        <v>9.2322797262964999E-4</v>
+      </c>
+      <c r="Z45" s="4">
+        <v>5.0740876061628774E-3</v>
+      </c>
+      <c r="AD45" s="2">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="AE45" s="4"/>
+      <c r="AF45" s="4"/>
+    </row>
+    <row r="46" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1981,10 +2800,30 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-    </row>
-    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T46" s="3">
+        <v>1.2951348519433581</v>
+      </c>
+      <c r="U46" s="3">
+        <v>1.922531464144752</v>
+      </c>
+      <c r="X46" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="Y46" s="4">
+        <v>8.3189701341573408E-4</v>
+      </c>
+      <c r="Z46" s="4">
+        <v>7.9173543524065151E-3</v>
+      </c>
+      <c r="AD46" s="2">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+    </row>
+    <row r="47" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2019,10 +2858,30 @@
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-    </row>
-    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T47" s="3">
+        <v>1.1034291689922651</v>
+      </c>
+      <c r="U47" s="3">
+        <v>2.1178467203924849</v>
+      </c>
+      <c r="X47" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="Y47" s="4">
+        <v>8.4725194294970696E-4</v>
+      </c>
+      <c r="Z47" s="4">
+        <v>8.6944695513224059E-3</v>
+      </c>
+      <c r="AD47" s="2">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="AE47" s="4"/>
+      <c r="AF47" s="4"/>
+    </row>
+    <row r="48" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2057,10 +2916,30 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-    </row>
-    <row r="49" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T48" s="3">
+        <v>1.0640106702839871</v>
+      </c>
+      <c r="U48" s="3">
+        <v>1.778557935459985</v>
+      </c>
+      <c r="X48" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="Y48" s="4">
+        <v>9.2248137705867438E-4</v>
+      </c>
+      <c r="Z48" s="4">
+        <v>4.5614777306711802E-3</v>
+      </c>
+      <c r="AD48" s="2">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="AE48" s="4"/>
+      <c r="AF48" s="4"/>
+    </row>
+    <row r="49" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2095,10 +2974,30 @@
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-    </row>
-    <row r="50" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T49" s="3">
+        <v>1.27075671409364</v>
+      </c>
+      <c r="U49" s="3">
+        <v>2.8702320641634791</v>
+      </c>
+      <c r="X49" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="Y49" s="4">
+        <v>8.1927442868793329E-4</v>
+      </c>
+      <c r="Z49" s="4">
+        <v>7.5480578593691474E-3</v>
+      </c>
+      <c r="AD49" s="2">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="AE49" s="4"/>
+      <c r="AF49" s="4"/>
+    </row>
+    <row r="50" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2133,10 +3032,30 @@
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-    </row>
-    <row r="51" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T50" s="3">
+        <v>0.89078150602175188</v>
+      </c>
+      <c r="U50" s="3">
+        <v>4.9270642904264754</v>
+      </c>
+      <c r="X50" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="Y50" s="4">
+        <v>9.6845776757179078E-4</v>
+      </c>
+      <c r="Z50" s="4">
+        <v>4.514784686722886E-3</v>
+      </c>
+      <c r="AD50" s="2">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="AE50" s="4"/>
+      <c r="AF50" s="4"/>
+    </row>
+    <row r="51" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2171,10 +3090,30 @@
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-    </row>
-    <row r="52" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T51" s="3">
+        <v>1.065583385785051</v>
+      </c>
+      <c r="U51" s="3">
+        <v>4.4196225895728674</v>
+      </c>
+      <c r="X51" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="Y51" s="4">
+        <v>8.2732407862393781E-4</v>
+      </c>
+      <c r="Z51" s="4">
+        <v>8.2313946872629527E-3</v>
+      </c>
+      <c r="AD51" s="2">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="AE51" s="4"/>
+      <c r="AF51" s="4"/>
+    </row>
+    <row r="52" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2209,10 +3148,30 @@
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-    </row>
-    <row r="53" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T52" s="3">
+        <v>1.1818609064173879</v>
+      </c>
+      <c r="U52" s="3">
+        <v>2.113238580387617</v>
+      </c>
+      <c r="X52" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="Y52" s="4">
+        <v>9.239102621895587E-4</v>
+      </c>
+      <c r="Z52" s="4">
+        <v>5.6084003604215463E-3</v>
+      </c>
+      <c r="AD52" s="2">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="AE52" s="4"/>
+      <c r="AF52" s="4"/>
+    </row>
+    <row r="53" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2247,10 +3206,30 @@
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-    </row>
-    <row r="54" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T53" s="3">
+        <v>1.1619450499015631</v>
+      </c>
+      <c r="U53" s="3">
+        <v>3.0256401956818721</v>
+      </c>
+      <c r="X53" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="Y53" s="4">
+        <v>9.6177525790612094E-4</v>
+      </c>
+      <c r="Z53" s="4">
+        <v>5.2829536118410899E-3</v>
+      </c>
+      <c r="AD53" s="2">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="AE53" s="4"/>
+      <c r="AF53" s="4"/>
+    </row>
+    <row r="54" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2285,10 +3264,30 @@
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-    </row>
-    <row r="55" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T54" s="3">
+        <v>1.2506853131901201</v>
+      </c>
+      <c r="U54" s="3">
+        <v>2.2757036192265012</v>
+      </c>
+      <c r="X54" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="Y54" s="4">
+        <v>9.19886194547712E-4</v>
+      </c>
+      <c r="Z54" s="4">
+        <v>4.7247065064285367E-3</v>
+      </c>
+      <c r="AD54" s="2">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="AE54" s="4"/>
+      <c r="AF54" s="4"/>
+    </row>
+    <row r="55" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2323,10 +3322,30 @@
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-    </row>
-    <row r="56" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T55" s="3">
+        <v>0.95237250065534895</v>
+      </c>
+      <c r="U55" s="3">
+        <v>3.5239536909862208</v>
+      </c>
+      <c r="X55" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="Y55" s="4">
+        <v>8.8049758828907766E-4</v>
+      </c>
+      <c r="Z55" s="4">
+        <v>5.9240492335451431E-3</v>
+      </c>
+      <c r="AD55" s="2">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="AE55" s="4"/>
+      <c r="AF55" s="4"/>
+    </row>
+    <row r="56" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D56" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2361,10 +3380,30 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-    </row>
-    <row r="58" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="T56" s="3">
+        <v>0.96892165852051226</v>
+      </c>
+      <c r="U56" s="3">
+        <v>3.9102526621760472</v>
+      </c>
+      <c r="X56" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="Y56" s="4">
+        <v>9.1830921364576522E-4</v>
+      </c>
+      <c r="Z56" s="4">
+        <v>4.9328516840289769E-3</v>
+      </c>
+      <c r="AD56" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="AE56" s="4"/>
+      <c r="AF56" s="4"/>
+    </row>
+    <row r="58" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>4</v>
       </c>
@@ -2401,16 +3440,38 @@
       <c r="S58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="T58" s="3" t="e">
+      <c r="T58" s="3">
         <f>AVERAGE(T7:T56)</f>
+        <v>1.0871327423415438</v>
+      </c>
+      <c r="U58" s="3">
+        <f>AVERAGE(U7:U56)</f>
+        <v>3.0838451417512793</v>
+      </c>
+      <c r="X58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y58" s="4">
+        <f>AVERAGE(Y7:Y56)</f>
+        <v>8.8132614522225673E-4</v>
+      </c>
+      <c r="Z58" s="4">
+        <f>AVERAGE(Z7:Z56)</f>
+        <v>6.3054894442772114E-3</v>
+      </c>
+      <c r="AD58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE58" s="4" t="e">
+        <f>AVERAGE(AE7:AE56)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U58" s="3" t="e">
-        <f>AVERAGE(U7:U56)</f>
+      <c r="AF58" s="4" t="e">
+        <f>AVERAGE(AF7:AF56)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="59" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>5</v>
       </c>
@@ -2447,12 +3508,34 @@
       <c r="S59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="T59" s="3" t="e">
+      <c r="T59" s="3">
         <f>_xlfn.STDEV.S(T7:T56)</f>
+        <v>0.15211956374222982</v>
+      </c>
+      <c r="U59" s="3">
+        <f>_xlfn.STDEV.S(U7:U56)</f>
+        <v>1.3553488098915927</v>
+      </c>
+      <c r="X59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y59" s="4">
+        <f>_xlfn.STDEV.S(Y7:Y56)</f>
+        <v>5.2597398990294191E-5</v>
+      </c>
+      <c r="Z59" s="4">
+        <f>_xlfn.STDEV.S(Z7:Z56)</f>
+        <v>1.3820977348093018E-3</v>
+      </c>
+      <c r="AD59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE59" s="4" t="e">
+        <f>_xlfn.STDEV.S(AE7:AE56)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U59" s="3" t="e">
-        <f>_xlfn.STDEV.S(U7:U56)</f>
+      <c r="AF59" s="4" t="e">
+        <f>_xlfn.STDEV.S(AF7:AF56)</f>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test-1 for hybrid model (MSE)
</commit_message>
<xml_diff>
--- a/migforecasting/Hybridization/exp/test 1.xlsx
+++ b/migforecasting/Hybridization/exp/test 1.xlsx
@@ -399,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D4:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,8 +558,12 @@
       <c r="AD7" s="2">
         <v>1</v>
       </c>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
+      <c r="AE7" s="4">
+        <v>8.6340456197939001E-4</v>
+      </c>
+      <c r="AF7" s="4">
+        <v>6.0508952270225871E-3</v>
+      </c>
     </row>
     <row r="8" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D8" s="2">
@@ -616,8 +620,12 @@
         <f>AD7+1</f>
         <v>2</v>
       </c>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
+      <c r="AE8" s="4">
+        <v>8.4502880735631326E-4</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>6.2916040116183913E-3</v>
+      </c>
     </row>
     <row r="9" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
@@ -674,8 +682,12 @@
         <f t="shared" ref="AD9:AD56" si="5">AD8+1</f>
         <v>3</v>
       </c>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
+      <c r="AE9" s="4">
+        <v>7.7195715375899098E-4</v>
+      </c>
+      <c r="AF9" s="4">
+        <v>7.5465539279952814E-3</v>
+      </c>
     </row>
     <row r="10" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D10" s="2">
@@ -732,8 +744,12 @@
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="AE10" s="4"/>
-      <c r="AF10" s="4"/>
+      <c r="AE10" s="4">
+        <v>7.1656105194302497E-4</v>
+      </c>
+      <c r="AF10" s="4">
+        <v>8.5826796550299914E-3</v>
+      </c>
     </row>
     <row r="11" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D11" s="2">
@@ -790,8 +806,12 @@
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="4"/>
+      <c r="AE11" s="4">
+        <v>8.258253827837721E-4</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>7.1834017823041076E-3</v>
+      </c>
     </row>
     <row r="12" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D12" s="2">
@@ -848,8 +868,12 @@
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="AE12" s="4"/>
-      <c r="AF12" s="4"/>
+      <c r="AE12" s="4">
+        <v>7.3775063817157192E-4</v>
+      </c>
+      <c r="AF12" s="4">
+        <v>8.128328808893125E-3</v>
+      </c>
     </row>
     <row r="13" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D13" s="2">
@@ -906,8 +930,12 @@
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="AE13" s="4"/>
-      <c r="AF13" s="4"/>
+      <c r="AE13" s="4">
+        <v>8.0877247988693827E-4</v>
+      </c>
+      <c r="AF13" s="4">
+        <v>6.9513280399387508E-3</v>
+      </c>
     </row>
     <row r="14" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D14" s="2">
@@ -964,8 +992,12 @@
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
+      <c r="AE14" s="4">
+        <v>8.7919170260952035E-4</v>
+      </c>
+      <c r="AF14" s="4">
+        <v>6.3668778389247126E-3</v>
+      </c>
     </row>
     <row r="15" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D15" s="2">
@@ -1022,8 +1054,12 @@
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
+      <c r="AE15" s="4">
+        <v>8.9660909912945273E-4</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>5.7842425560125079E-3</v>
+      </c>
     </row>
     <row r="16" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D16" s="2">
@@ -1080,8 +1116,12 @@
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
+      <c r="AE16" s="4">
+        <v>7.9600310500722534E-4</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>6.8676535962152859E-3</v>
+      </c>
     </row>
     <row r="17" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D17" s="2">
@@ -1138,8 +1178,12 @@
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
+      <c r="AE17" s="4">
+        <v>8.7669525616632961E-4</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>4.7843640386389932E-3</v>
+      </c>
     </row>
     <row r="18" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D18" s="2">
@@ -1196,8 +1240,12 @@
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
+      <c r="AE18" s="4">
+        <v>7.1118319664440844E-4</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>9.0907566776924093E-3</v>
+      </c>
     </row>
     <row r="19" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D19" s="2">
@@ -1254,8 +1302,12 @@
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="AE19" s="4"/>
-      <c r="AF19" s="4"/>
+      <c r="AE19" s="4">
+        <v>8.8649397116871383E-4</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>4.8687011248475078E-3</v>
+      </c>
     </row>
     <row r="20" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D20" s="2">
@@ -1312,8 +1364,12 @@
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
-      <c r="AE20" s="4"/>
-      <c r="AF20" s="4"/>
+      <c r="AE20" s="4">
+        <v>9.1672137200346645E-4</v>
+      </c>
+      <c r="AF20" s="4">
+        <v>6.4773981117315976E-3</v>
+      </c>
     </row>
     <row r="21" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D21" s="2">
@@ -1370,8 +1426,12 @@
         <f t="shared" si="5"/>
         <v>15</v>
       </c>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="4"/>
+      <c r="AE21" s="4">
+        <v>8.0614299716547143E-4</v>
+      </c>
+      <c r="AF21" s="4">
+        <v>6.2370259912589614E-3</v>
+      </c>
     </row>
     <row r="22" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D22" s="2">
@@ -1428,8 +1488,12 @@
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="AE22" s="4"/>
-      <c r="AF22" s="4"/>
+      <c r="AE22" s="4">
+        <v>7.9080541135545805E-4</v>
+      </c>
+      <c r="AF22" s="4">
+        <v>6.5147986790045501E-3</v>
+      </c>
     </row>
     <row r="23" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D23" s="2">
@@ -1486,8 +1550,12 @@
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="AE23" s="4"/>
-      <c r="AF23" s="4"/>
+      <c r="AE23" s="4">
+        <v>8.6468352780674372E-4</v>
+      </c>
+      <c r="AF23" s="4">
+        <v>5.9362376625253909E-3</v>
+      </c>
     </row>
     <row r="24" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D24" s="2">
@@ -1544,8 +1612,12 @@
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="AE24" s="4"/>
-      <c r="AF24" s="4"/>
+      <c r="AE24" s="4">
+        <v>8.5599131157726275E-4</v>
+      </c>
+      <c r="AF24" s="4">
+        <v>5.8520156098341028E-3</v>
+      </c>
     </row>
     <row r="25" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D25" s="2">
@@ -1602,8 +1674,12 @@
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
+      <c r="AE25" s="4">
+        <v>8.4265711138683326E-4</v>
+      </c>
+      <c r="AF25" s="4">
+        <v>5.4908804671530854E-3</v>
+      </c>
     </row>
     <row r="26" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D26" s="2">
@@ -1660,8 +1736,12 @@
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="AE26" s="4"/>
-      <c r="AF26" s="4"/>
+      <c r="AE26" s="4">
+        <v>8.3578475464690725E-4</v>
+      </c>
+      <c r="AF26" s="4">
+        <v>6.116356639690265E-3</v>
+      </c>
     </row>
     <row r="27" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D27" s="2">
@@ -1718,8 +1798,12 @@
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
-      <c r="AE27" s="4"/>
-      <c r="AF27" s="4"/>
+      <c r="AE27" s="4">
+        <v>9.2388903199000028E-4</v>
+      </c>
+      <c r="AF27" s="4">
+        <v>4.9288637436241522E-3</v>
+      </c>
     </row>
     <row r="28" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D28" s="2">
@@ -1776,8 +1860,12 @@
         <f t="shared" si="5"/>
         <v>22</v>
       </c>
-      <c r="AE28" s="4"/>
-      <c r="AF28" s="4"/>
+      <c r="AE28" s="4">
+        <v>9.1465408536584828E-4</v>
+      </c>
+      <c r="AF28" s="4">
+        <v>5.8741727440370546E-3</v>
+      </c>
     </row>
     <row r="29" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D29" s="2">
@@ -1834,8 +1922,12 @@
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="AE29" s="4"/>
-      <c r="AF29" s="4"/>
+      <c r="AE29" s="4">
+        <v>8.5927450294244446E-4</v>
+      </c>
+      <c r="AF29" s="4">
+        <v>6.6957295723573153E-3</v>
+      </c>
     </row>
     <row r="30" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D30" s="2">
@@ -1892,8 +1984,12 @@
         <f t="shared" si="5"/>
         <v>24</v>
       </c>
-      <c r="AE30" s="4"/>
-      <c r="AF30" s="4"/>
+      <c r="AE30" s="4">
+        <v>8.4046554404440391E-4</v>
+      </c>
+      <c r="AF30" s="4">
+        <v>6.0809824661571896E-3</v>
+      </c>
     </row>
     <row r="31" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D31" s="2">
@@ -1950,8 +2046,12 @@
         <f t="shared" si="5"/>
         <v>25</v>
       </c>
-      <c r="AE31" s="4"/>
-      <c r="AF31" s="4"/>
+      <c r="AE31" s="4">
+        <v>8.3500849125374389E-4</v>
+      </c>
+      <c r="AF31" s="4">
+        <v>5.9186252738086063E-3</v>
+      </c>
     </row>
     <row r="32" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D32" s="2">
@@ -2008,8 +2108,12 @@
         <f t="shared" si="5"/>
         <v>26</v>
       </c>
-      <c r="AE32" s="4"/>
-      <c r="AF32" s="4"/>
+      <c r="AE32" s="4">
+        <v>7.8665944380502993E-4</v>
+      </c>
+      <c r="AF32" s="4">
+        <v>8.9802493366992076E-3</v>
+      </c>
     </row>
     <row r="33" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D33" s="2">
@@ -2066,8 +2170,12 @@
         <f t="shared" si="5"/>
         <v>27</v>
       </c>
-      <c r="AE33" s="4"/>
-      <c r="AF33" s="4"/>
+      <c r="AE33" s="4">
+        <v>8.4625978788563079E-4</v>
+      </c>
+      <c r="AF33" s="4">
+        <v>6.6392515850746984E-3</v>
+      </c>
     </row>
     <row r="34" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D34" s="2">
@@ -2124,8 +2232,12 @@
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
-      <c r="AE34" s="4"/>
-      <c r="AF34" s="4"/>
+      <c r="AE34" s="4">
+        <v>8.1680227774547228E-4</v>
+      </c>
+      <c r="AF34" s="4">
+        <v>6.3967235053326516E-3</v>
+      </c>
     </row>
     <row r="35" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D35" s="2">
@@ -2182,8 +2294,12 @@
         <f t="shared" si="5"/>
         <v>29</v>
       </c>
-      <c r="AE35" s="4"/>
-      <c r="AF35" s="4"/>
+      <c r="AE35" s="4">
+        <v>7.8342656647699784E-4</v>
+      </c>
+      <c r="AF35" s="4">
+        <v>7.9021173219589545E-3</v>
+      </c>
     </row>
     <row r="36" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D36" s="2">
@@ -2240,8 +2356,12 @@
         <f t="shared" si="5"/>
         <v>30</v>
       </c>
-      <c r="AE36" s="4"/>
-      <c r="AF36" s="4"/>
+      <c r="AE36" s="4">
+        <v>8.9574455591543778E-4</v>
+      </c>
+      <c r="AF36" s="4">
+        <v>5.1729644095041974E-3</v>
+      </c>
     </row>
     <row r="37" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D37" s="2">
@@ -2298,8 +2418,12 @@
         <f t="shared" si="5"/>
         <v>31</v>
       </c>
-      <c r="AE37" s="4"/>
-      <c r="AF37" s="4"/>
+      <c r="AE37" s="4">
+        <v>8.2280602136381863E-4</v>
+      </c>
+      <c r="AF37" s="4">
+        <v>6.1684486282195536E-3</v>
+      </c>
     </row>
     <row r="38" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D38" s="2">
@@ -2356,8 +2480,12 @@
         <f t="shared" si="5"/>
         <v>32</v>
       </c>
-      <c r="AE38" s="4"/>
-      <c r="AF38" s="4"/>
+      <c r="AE38" s="4">
+        <v>7.4071045141117504E-4</v>
+      </c>
+      <c r="AF38" s="4">
+        <v>1.092020314707156E-2</v>
+      </c>
     </row>
     <row r="39" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D39" s="2">
@@ -2414,8 +2542,12 @@
         <f t="shared" si="5"/>
         <v>33</v>
       </c>
-      <c r="AE39" s="4"/>
-      <c r="AF39" s="4"/>
+      <c r="AE39" s="4">
+        <v>8.275783140295305E-4</v>
+      </c>
+      <c r="AF39" s="4">
+        <v>7.2648345874836507E-3</v>
+      </c>
     </row>
     <row r="40" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D40" s="2">
@@ -2472,8 +2604,12 @@
         <f t="shared" si="5"/>
         <v>34</v>
       </c>
-      <c r="AE40" s="4"/>
-      <c r="AF40" s="4"/>
+      <c r="AE40" s="4">
+        <v>8.4922984534872023E-4</v>
+      </c>
+      <c r="AF40" s="4">
+        <v>4.8028738161044627E-3</v>
+      </c>
     </row>
     <row r="41" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D41" s="2">
@@ -2530,8 +2666,12 @@
         <f t="shared" si="5"/>
         <v>35</v>
       </c>
-      <c r="AE41" s="4"/>
-      <c r="AF41" s="4"/>
+      <c r="AE41" s="4">
+        <v>7.6550630249273984E-4</v>
+      </c>
+      <c r="AF41" s="4">
+        <v>8.7473283883004634E-3</v>
+      </c>
     </row>
     <row r="42" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D42" s="2">
@@ -2588,8 +2728,12 @@
         <f t="shared" si="5"/>
         <v>36</v>
       </c>
-      <c r="AE42" s="4"/>
-      <c r="AF42" s="4"/>
+      <c r="AE42" s="4">
+        <v>8.4673677432635093E-4</v>
+      </c>
+      <c r="AF42" s="4">
+        <v>8.8404739987928554E-3</v>
+      </c>
     </row>
     <row r="43" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D43" s="2">
@@ -2646,8 +2790,12 @@
         <f t="shared" si="5"/>
         <v>37</v>
       </c>
-      <c r="AE43" s="4"/>
-      <c r="AF43" s="4"/>
+      <c r="AE43" s="4">
+        <v>8.0062766421530097E-4</v>
+      </c>
+      <c r="AF43" s="4">
+        <v>7.1022060823421884E-3</v>
+      </c>
     </row>
     <row r="44" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D44" s="2">
@@ -2704,8 +2852,12 @@
         <f t="shared" si="5"/>
         <v>38</v>
       </c>
-      <c r="AE44" s="4"/>
-      <c r="AF44" s="4"/>
+      <c r="AE44" s="4">
+        <v>9.0191750943323617E-4</v>
+      </c>
+      <c r="AF44" s="4">
+        <v>5.2808735303675096E-3</v>
+      </c>
     </row>
     <row r="45" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D45" s="2">
@@ -2762,8 +2914,12 @@
         <f t="shared" si="5"/>
         <v>39</v>
       </c>
-      <c r="AE45" s="4"/>
-      <c r="AF45" s="4"/>
+      <c r="AE45" s="4">
+        <v>8.2095438099731143E-4</v>
+      </c>
+      <c r="AF45" s="4">
+        <v>5.9319828540863196E-3</v>
+      </c>
     </row>
     <row r="46" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D46" s="2">
@@ -2820,8 +2976,12 @@
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="AE46" s="4"/>
-      <c r="AF46" s="4"/>
+      <c r="AE46" s="4">
+        <v>8.4893170328617694E-4</v>
+      </c>
+      <c r="AF46" s="4">
+        <v>6.881284501036462E-3</v>
+      </c>
     </row>
     <row r="47" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D47" s="2">
@@ -2878,8 +3038,12 @@
         <f t="shared" si="5"/>
         <v>41</v>
       </c>
-      <c r="AE47" s="4"/>
-      <c r="AF47" s="4"/>
+      <c r="AE47" s="4">
+        <v>7.4947183422892686E-4</v>
+      </c>
+      <c r="AF47" s="4">
+        <v>6.6485166380760401E-3</v>
+      </c>
     </row>
     <row r="48" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D48" s="2">
@@ -2936,8 +3100,12 @@
         <f t="shared" si="5"/>
         <v>42</v>
       </c>
-      <c r="AE48" s="4"/>
-      <c r="AF48" s="4"/>
+      <c r="AE48" s="4">
+        <v>9.1886300042368888E-4</v>
+      </c>
+      <c r="AF48" s="4">
+        <v>5.6748862313427103E-3</v>
+      </c>
     </row>
     <row r="49" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D49" s="2">
@@ -2994,8 +3162,12 @@
         <f t="shared" si="5"/>
         <v>43</v>
       </c>
-      <c r="AE49" s="4"/>
-      <c r="AF49" s="4"/>
+      <c r="AE49" s="4">
+        <v>8.7664367090482158E-4</v>
+      </c>
+      <c r="AF49" s="4">
+        <v>5.1514372111189401E-3</v>
+      </c>
     </row>
     <row r="50" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D50" s="2">
@@ -3052,8 +3224,12 @@
         <f t="shared" si="5"/>
         <v>44</v>
       </c>
-      <c r="AE50" s="4"/>
-      <c r="AF50" s="4"/>
+      <c r="AE50" s="4">
+        <v>8.1896554455745951E-4</v>
+      </c>
+      <c r="AF50" s="4">
+        <v>6.4955108341278071E-3</v>
+      </c>
     </row>
     <row r="51" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D51" s="2">
@@ -3110,8 +3286,12 @@
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="AE51" s="4"/>
-      <c r="AF51" s="4"/>
+      <c r="AE51" s="4">
+        <v>9.2376417485305227E-4</v>
+      </c>
+      <c r="AF51" s="4">
+        <v>3.836989199788257E-3</v>
+      </c>
     </row>
     <row r="52" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D52" s="2">
@@ -3168,8 +3348,12 @@
         <f t="shared" si="5"/>
         <v>46</v>
       </c>
-      <c r="AE52" s="4"/>
-      <c r="AF52" s="4"/>
+      <c r="AE52" s="4">
+        <v>8.1643309895520577E-4</v>
+      </c>
+      <c r="AF52" s="4">
+        <v>6.7955937328387853E-3</v>
+      </c>
     </row>
     <row r="53" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D53" s="2">
@@ -3226,8 +3410,12 @@
         <f t="shared" si="5"/>
         <v>47</v>
       </c>
-      <c r="AE53" s="4"/>
-      <c r="AF53" s="4"/>
+      <c r="AE53" s="4">
+        <v>9.1906258262140707E-4</v>
+      </c>
+      <c r="AF53" s="4">
+        <v>5.3889365434957107E-3</v>
+      </c>
     </row>
     <row r="54" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D54" s="2">
@@ -3284,8 +3472,12 @@
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
-      <c r="AE54" s="4"/>
-      <c r="AF54" s="4"/>
+      <c r="AE54" s="4">
+        <v>8.3007365733830734E-4</v>
+      </c>
+      <c r="AF54" s="4">
+        <v>6.8132953316198076E-3</v>
+      </c>
     </row>
     <row r="55" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D55" s="2">
@@ -3342,8 +3534,12 @@
         <f t="shared" si="5"/>
         <v>49</v>
       </c>
-      <c r="AE55" s="4"/>
-      <c r="AF55" s="4"/>
+      <c r="AE55" s="4">
+        <v>7.3253315661487184E-4</v>
+      </c>
+      <c r="AF55" s="4">
+        <v>8.0311434514602452E-3</v>
+      </c>
     </row>
     <row r="56" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D56" s="2">
@@ -3400,8 +3596,12 @@
         <f t="shared" si="5"/>
         <v>50</v>
       </c>
-      <c r="AE56" s="4"/>
-      <c r="AF56" s="4"/>
+      <c r="AE56" s="4">
+        <v>7.9339724802980139E-4</v>
+      </c>
+      <c r="AF56" s="4">
+        <v>6.2239485711956134E-3</v>
+      </c>
     </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
@@ -3462,13 +3662,13 @@
       <c r="AD58" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="AE58" s="4" t="e">
+      <c r="AE58" s="4">
         <f>AVERAGE(AE7:AE56)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF58" s="4" t="e">
+        <v>8.3269308230809395E-4</v>
+      </c>
+      <c r="AF58" s="4">
         <f>AVERAGE(AF7:AF56)</f>
-        <v>#DIV/0!</v>
+        <v>6.5742509536750905E-3</v>
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.25">
@@ -3530,13 +3730,13 @@
       <c r="AD59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="AE59" s="4" t="e">
+      <c r="AE59" s="4">
         <f>_xlfn.STDEV.S(AE7:AE56)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AF59" s="4" t="e">
+        <v>5.6227823936768716E-5</v>
+      </c>
+      <c r="AF59" s="4">
         <f>_xlfn.STDEV.S(AF7:AF56)</f>
-        <v>#DIV/0!</v>
+        <v>1.3279746778569084E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test-1 more repeats for MAE
</commit_message>
<xml_diff>
--- a/migforecasting/Hybridization/exp/test 1.xlsx
+++ b/migforecasting/Hybridization/exp/test 1.xlsx
@@ -397,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:AF59"/>
+  <dimension ref="D4:AF111"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L87" sqref="L87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="9" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D9" s="2">
-        <f t="shared" ref="D9:D56" si="0">D8+1</f>
+        <f t="shared" ref="D9:D72" si="0">D8+1</f>
         <v>3</v>
       </c>
       <c r="E9" s="3">
@@ -639,7 +639,7 @@
         <v>1200.3342958830549</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" ref="I9:I56" si="1">I8+1</f>
+        <f t="shared" ref="I9:I72" si="1">I8+1</f>
         <v>3</v>
       </c>
       <c r="J9" s="3">
@@ -3603,28 +3603,48 @@
         <v>6.2239485711956134E-3</v>
       </c>
     </row>
+    <row r="57" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D57" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="E57" s="3">
+        <v>469.59099924584177</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1121.3643217401141</v>
+      </c>
+      <c r="I57" s="2">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="J57" s="3">
+        <v>459.78722056477659</v>
+      </c>
+      <c r="K57" s="3">
+        <v>1216.2028116100801</v>
+      </c>
+    </row>
     <row r="58" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D58" s="2" t="s">
-        <v>4</v>
+      <c r="D58" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="E58" s="3">
-        <f>AVERAGE(E7:E56)</f>
-        <v>465.99822623802623</v>
+        <v>462.90276812930392</v>
       </c>
       <c r="F58" s="3">
-        <f>AVERAGE(F7:F56)</f>
-        <v>1243.4855411336976</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>4</v>
+        <v>1321.186205651466</v>
+      </c>
+      <c r="I58" s="2">
+        <f t="shared" si="1"/>
+        <v>52</v>
       </c>
       <c r="J58" s="3">
-        <f>AVERAGE(J7:J56)</f>
-        <v>447.60930906114072</v>
+        <v>456.8964202900641</v>
       </c>
       <c r="K58" s="3">
-        <f>AVERAGE(K7:K56)</f>
-        <v>1243.9082469044483</v>
+        <v>1026.089991348555</v>
       </c>
       <c r="N58" s="2" t="s">
         <v>4</v>
@@ -3672,27 +3692,25 @@
       </c>
     </row>
     <row r="59" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D59" s="2" t="s">
-        <v>5</v>
+      <c r="D59" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="E59" s="3">
-        <f>_xlfn.STDEV.S(E7:E56)</f>
-        <v>9.7163393380093197</v>
+        <v>474.79970889021729</v>
       </c>
       <c r="F59" s="3">
-        <f>_xlfn.STDEV.S(F7:F56)</f>
-        <v>76.67452985223207</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>5</v>
+        <v>1169.5232512226321</v>
+      </c>
+      <c r="I59" s="2">
+        <f t="shared" si="1"/>
+        <v>53</v>
       </c>
       <c r="J59" s="3">
-        <f>_xlfn.STDEV.S(J7:J56)</f>
-        <v>9.0109446368246164</v>
+        <v>443.86080241695993</v>
       </c>
       <c r="K59" s="3">
-        <f>_xlfn.STDEV.S(K7:K56)</f>
-        <v>71.799520250849241</v>
+        <v>1286.1540621663751</v>
       </c>
       <c r="N59" s="2" t="s">
         <v>5</v>
@@ -3739,7 +3757,1090 @@
         <v>1.3279746778569084E-3</v>
       </c>
     </row>
+    <row r="60" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D60" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E60" s="3">
+        <v>467.81306704380012</v>
+      </c>
+      <c r="F60" s="3">
+        <v>1188.46641104272</v>
+      </c>
+      <c r="I60" s="2">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="J60" s="3">
+        <v>470.72997825737713</v>
+      </c>
+      <c r="K60" s="3">
+        <v>1054.4750573439389</v>
+      </c>
+    </row>
+    <row r="61" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D61" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="E61" s="3">
+        <v>478.84603896941962</v>
+      </c>
+      <c r="F61" s="3">
+        <v>1110.3296882440061</v>
+      </c>
+      <c r="I61" s="2">
+        <f t="shared" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="J61" s="3">
+        <v>446.43752674024898</v>
+      </c>
+      <c r="K61" s="3">
+        <v>1231.3058978412109</v>
+      </c>
+    </row>
+    <row r="62" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D62" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E62" s="3">
+        <v>478.00944234136273</v>
+      </c>
+      <c r="F62" s="3">
+        <v>1125.0784059880391</v>
+      </c>
+      <c r="I62" s="2">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="J62" s="3">
+        <v>429.6367946729323</v>
+      </c>
+      <c r="K62" s="3">
+        <v>1324.802861360447</v>
+      </c>
+    </row>
+    <row r="63" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D63" s="2">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="E63" s="3">
+        <v>467.51460264292592</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1160.672379335753</v>
+      </c>
+      <c r="I63" s="2">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="J63" s="3">
+        <v>453.62032936299141</v>
+      </c>
+      <c r="K63" s="3">
+        <v>1150.983723921031</v>
+      </c>
+    </row>
+    <row r="64" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D64" s="2">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="E64" s="3">
+        <v>460.22378714358592</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1208.347679236289</v>
+      </c>
+      <c r="I64" s="2">
+        <f t="shared" si="1"/>
+        <v>58</v>
+      </c>
+      <c r="J64" s="3">
+        <v>453.20647232376479</v>
+      </c>
+      <c r="K64" s="3">
+        <v>1177.4578174891719</v>
+      </c>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D65" s="2">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="E65" s="3">
+        <v>454.29498047376939</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1469.198687308944</v>
+      </c>
+      <c r="I65" s="2">
+        <f t="shared" si="1"/>
+        <v>59</v>
+      </c>
+      <c r="J65" s="3">
+        <v>438.82059956895063</v>
+      </c>
+      <c r="K65" s="3">
+        <v>1257.5500300216679</v>
+      </c>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D66" s="2">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E66" s="3">
+        <v>463.97295434353288</v>
+      </c>
+      <c r="F66" s="3">
+        <v>1250.151977751864</v>
+      </c>
+      <c r="I66" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J66" s="3">
+        <v>454.41435147459549</v>
+      </c>
+      <c r="K66" s="3">
+        <v>1275.0452510378079</v>
+      </c>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D67" s="2">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="E67" s="3">
+        <v>448.64057347263088</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1376.99634606265</v>
+      </c>
+      <c r="I67" s="2">
+        <f t="shared" si="1"/>
+        <v>61</v>
+      </c>
+      <c r="J67" s="3">
+        <v>454.60655401507029</v>
+      </c>
+      <c r="K67" s="3">
+        <v>1113.9531020019299</v>
+      </c>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D68" s="2">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="E68" s="3">
+        <v>461.62809542571478</v>
+      </c>
+      <c r="F68" s="3">
+        <v>1305.7403361599979</v>
+      </c>
+      <c r="I68" s="2">
+        <f t="shared" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="J68" s="3">
+        <v>445.55718154273302</v>
+      </c>
+      <c r="K68" s="3">
+        <v>1279.6359239596979</v>
+      </c>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D69" s="2">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="E69" s="3">
+        <v>470.06574602842232</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1250.7112331196511</v>
+      </c>
+      <c r="I69" s="2">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="J69" s="3">
+        <v>459.78316840468551</v>
+      </c>
+      <c r="K69" s="3">
+        <v>1200.081566306666</v>
+      </c>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D70" s="2">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="E70" s="3">
+        <v>460.66879348629362</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1267.9817490083969</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="J70" s="3">
+        <v>447.63658372134518</v>
+      </c>
+      <c r="K70" s="3">
+        <v>1185.915864372341</v>
+      </c>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D71" s="2">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="E71" s="3">
+        <v>455.36676340008728</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1401.7729893689971</v>
+      </c>
+      <c r="I71" s="2">
+        <f t="shared" si="1"/>
+        <v>65</v>
+      </c>
+      <c r="J71" s="3">
+        <v>451.9582661293793</v>
+      </c>
+      <c r="K71" s="3">
+        <v>1290.5556438061001</v>
+      </c>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D72" s="2">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="E72" s="3">
+        <v>451.17076504361688</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1419.269336726629</v>
+      </c>
+      <c r="I72" s="2">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="J72" s="3">
+        <v>440.54146608600212</v>
+      </c>
+      <c r="K72" s="3">
+        <v>1275.1715890083481</v>
+      </c>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D73" s="2">
+        <f t="shared" ref="D73:D106" si="6">D72+1</f>
+        <v>67</v>
+      </c>
+      <c r="E73" s="3">
+        <v>477.95346349401319</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1082.26302826098</v>
+      </c>
+      <c r="I73" s="2">
+        <f t="shared" ref="I73:I106" si="7">I72+1</f>
+        <v>67</v>
+      </c>
+      <c r="J73" s="3">
+        <v>450.86867785060872</v>
+      </c>
+      <c r="K73" s="3">
+        <v>1249.830487709233</v>
+      </c>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D74" s="2">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+      <c r="E74" s="3">
+        <v>451.24021531060703</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1371.822335519196</v>
+      </c>
+      <c r="I74" s="2">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="J74" s="3">
+        <v>454.92770112002972</v>
+      </c>
+      <c r="K74" s="3">
+        <v>1207.3416149262041</v>
+      </c>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D75" s="2">
+        <f t="shared" si="6"/>
+        <v>69</v>
+      </c>
+      <c r="E75" s="3">
+        <v>460.77122457945461</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1207.2681613704181</v>
+      </c>
+      <c r="I75" s="2">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="J75" s="3">
+        <v>446.77573451261139</v>
+      </c>
+      <c r="K75" s="3">
+        <v>1208.9171253128011</v>
+      </c>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D76" s="2">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+      <c r="E76" s="3">
+        <v>475.38270335999692</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1257.392744477788</v>
+      </c>
+      <c r="I76" s="2">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="J76" s="3">
+        <v>457.62344758268028</v>
+      </c>
+      <c r="K76" s="3">
+        <v>1160.085019066008</v>
+      </c>
+    </row>
+    <row r="77" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D77" s="2">
+        <f t="shared" si="6"/>
+        <v>71</v>
+      </c>
+      <c r="E77" s="3">
+        <v>475.02511364971571</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1172.287615052662</v>
+      </c>
+      <c r="I77" s="2">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="J77" s="3">
+        <v>438.95018818537028</v>
+      </c>
+      <c r="K77" s="3">
+        <v>1333.405750395789</v>
+      </c>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D78" s="2">
+        <f t="shared" si="6"/>
+        <v>72</v>
+      </c>
+      <c r="E78" s="3">
+        <v>456.99960948602347</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1275.309699929232</v>
+      </c>
+      <c r="I78" s="2">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="J78" s="3">
+        <v>436.54559345058169</v>
+      </c>
+      <c r="K78" s="3">
+        <v>1406.8447173780339</v>
+      </c>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D79" s="2">
+        <f t="shared" si="6"/>
+        <v>73</v>
+      </c>
+      <c r="E79" s="3">
+        <v>466.95665910986799</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1209.592822936602</v>
+      </c>
+      <c r="I79" s="2">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="J79" s="3">
+        <v>448.36499975094648</v>
+      </c>
+      <c r="K79" s="3">
+        <v>1175.7383767506551</v>
+      </c>
+    </row>
+    <row r="80" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D80" s="2">
+        <f t="shared" si="6"/>
+        <v>74</v>
+      </c>
+      <c r="E80" s="3">
+        <v>470.94297830825252</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1191.942434971291</v>
+      </c>
+      <c r="I80" s="2">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+      <c r="J80" s="3">
+        <v>440.22202303512069</v>
+      </c>
+      <c r="K80" s="3">
+        <v>1168.9363468530139</v>
+      </c>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D81" s="2">
+        <f t="shared" si="6"/>
+        <v>75</v>
+      </c>
+      <c r="E81" s="3">
+        <v>464.49876907745892</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1224.4560788831791</v>
+      </c>
+      <c r="I81" s="2">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="J81" s="3">
+        <v>448.97515174398478</v>
+      </c>
+      <c r="K81" s="3">
+        <v>1251.0190193408121</v>
+      </c>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D82" s="2">
+        <f t="shared" si="6"/>
+        <v>76</v>
+      </c>
+      <c r="E82" s="3">
+        <v>454.3702272081743</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1355.4792545774219</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="J82" s="3">
+        <v>438.81177069034169</v>
+      </c>
+      <c r="K82" s="3">
+        <v>1307.3362279640471</v>
+      </c>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D83" s="2">
+        <f t="shared" si="6"/>
+        <v>77</v>
+      </c>
+      <c r="E83" s="3">
+        <v>480.37721877386753</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1193.7214377205421</v>
+      </c>
+      <c r="I83" s="2">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="J83" s="3">
+        <v>441.02512896255791</v>
+      </c>
+      <c r="K83" s="3">
+        <v>1357.937146251365</v>
+      </c>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D84" s="2">
+        <f t="shared" si="6"/>
+        <v>78</v>
+      </c>
+      <c r="E84" s="3">
+        <v>468.6764454981535</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1258.4734691381141</v>
+      </c>
+      <c r="I84" s="2">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="J84" s="3">
+        <v>460.68481427817647</v>
+      </c>
+      <c r="K84" s="3">
+        <v>1150.090320577671</v>
+      </c>
+    </row>
+    <row r="85" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D85" s="2">
+        <f t="shared" si="6"/>
+        <v>79</v>
+      </c>
+      <c r="E85" s="3">
+        <v>459.09994335252298</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1237.5365507912149</v>
+      </c>
+      <c r="I85" s="2">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+      <c r="J85" s="3">
+        <v>441.275859722625</v>
+      </c>
+      <c r="K85" s="3">
+        <v>1345.570372583614</v>
+      </c>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D86" s="2">
+        <f t="shared" si="6"/>
+        <v>80</v>
+      </c>
+      <c r="E86" s="3">
+        <v>475.01805591392821</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1275.0601616537331</v>
+      </c>
+      <c r="I86" s="2">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="J86" s="3">
+        <v>441.12654701569608</v>
+      </c>
+      <c r="K86" s="3">
+        <v>1213.594928794294</v>
+      </c>
+    </row>
+    <row r="87" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D87" s="2">
+        <f t="shared" si="6"/>
+        <v>81</v>
+      </c>
+      <c r="E87" s="3">
+        <v>470.29881232239751</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1165.775671724185</v>
+      </c>
+      <c r="I87" s="2">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="J87" s="3">
+        <v>442.96040439409268</v>
+      </c>
+      <c r="K87" s="3">
+        <v>1172.2340065612359</v>
+      </c>
+    </row>
+    <row r="88" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D88" s="2">
+        <f t="shared" si="6"/>
+        <v>82</v>
+      </c>
+      <c r="E88" s="3">
+        <v>466.9564645525125</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1196.674329661992</v>
+      </c>
+      <c r="I88" s="2">
+        <f t="shared" si="7"/>
+        <v>82</v>
+      </c>
+      <c r="J88" s="3">
+        <v>439.20440085121078</v>
+      </c>
+      <c r="K88" s="3">
+        <v>1195.4636734654171</v>
+      </c>
+    </row>
+    <row r="89" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D89" s="2">
+        <f t="shared" si="6"/>
+        <v>83</v>
+      </c>
+      <c r="E89" s="3">
+        <v>473.50539931148552</v>
+      </c>
+      <c r="F89" s="3">
+        <v>1170.3682755172019</v>
+      </c>
+      <c r="I89" s="2">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+      <c r="J89" s="3">
+        <v>444.73064151728607</v>
+      </c>
+      <c r="K89" s="3">
+        <v>1299.3285031359201</v>
+      </c>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D90" s="2">
+        <f t="shared" si="6"/>
+        <v>84</v>
+      </c>
+      <c r="E90" s="3">
+        <v>489.16856123087462</v>
+      </c>
+      <c r="F90" s="3">
+        <v>1115.866380747465</v>
+      </c>
+      <c r="I90" s="2">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+      <c r="J90" s="3">
+        <v>460.79071385936231</v>
+      </c>
+      <c r="K90" s="3">
+        <v>1072.6249777603759</v>
+      </c>
+    </row>
+    <row r="91" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D91" s="2">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+      <c r="E91" s="3">
+        <v>471.45319490937811</v>
+      </c>
+      <c r="F91" s="3">
+        <v>1319.5508382599351</v>
+      </c>
+      <c r="I91" s="2">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="J91" s="3">
+        <v>475.32850236434268</v>
+      </c>
+      <c r="K91" s="3">
+        <v>1043.893159491784</v>
+      </c>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D92" s="2">
+        <f t="shared" si="6"/>
+        <v>86</v>
+      </c>
+      <c r="E92" s="3">
+        <v>474.56695120446108</v>
+      </c>
+      <c r="F92" s="3">
+        <v>1129.9346809604981</v>
+      </c>
+      <c r="I92" s="2">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+      <c r="J92" s="3">
+        <v>451.91022388035373</v>
+      </c>
+      <c r="K92" s="3">
+        <v>1188.4247632252191</v>
+      </c>
+    </row>
+    <row r="93" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D93" s="2">
+        <f t="shared" si="6"/>
+        <v>87</v>
+      </c>
+      <c r="E93" s="3">
+        <v>464.13213580459058</v>
+      </c>
+      <c r="F93" s="3">
+        <v>1255.080606756273</v>
+      </c>
+      <c r="I93" s="2">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="J93" s="3">
+        <v>459.91654082622352</v>
+      </c>
+      <c r="K93" s="3">
+        <v>1099.2596286262501</v>
+      </c>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D94" s="2">
+        <f t="shared" si="6"/>
+        <v>88</v>
+      </c>
+      <c r="E94" s="3">
+        <v>465.09922674710072</v>
+      </c>
+      <c r="F94" s="3">
+        <v>1269.6717975975371</v>
+      </c>
+      <c r="I94" s="2">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="J94" s="3">
+        <v>460.61094957188209</v>
+      </c>
+      <c r="K94" s="3">
+        <v>1014.941892356086</v>
+      </c>
+    </row>
+    <row r="95" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D95" s="2">
+        <f t="shared" si="6"/>
+        <v>89</v>
+      </c>
+      <c r="E95" s="3">
+        <v>472.9816106576049</v>
+      </c>
+      <c r="F95" s="3">
+        <v>1199.997305236099</v>
+      </c>
+      <c r="I95" s="2">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+      <c r="J95" s="3">
+        <v>447.72978340343798</v>
+      </c>
+      <c r="K95" s="3">
+        <v>1361.93809894991</v>
+      </c>
+    </row>
+    <row r="96" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D96" s="2">
+        <f t="shared" si="6"/>
+        <v>90</v>
+      </c>
+      <c r="E96" s="3">
+        <v>447.63850245940148</v>
+      </c>
+      <c r="F96" s="3">
+        <v>1329.019374366188</v>
+      </c>
+      <c r="I96" s="2">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="J96" s="3">
+        <v>444.06555055241802</v>
+      </c>
+      <c r="K96" s="3">
+        <v>1309.5048107808061</v>
+      </c>
+    </row>
+    <row r="97" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D97" s="2">
+        <f t="shared" si="6"/>
+        <v>91</v>
+      </c>
+      <c r="E97" s="3">
+        <v>467.59260672467752</v>
+      </c>
+      <c r="F97" s="3">
+        <v>1311.0849874392941</v>
+      </c>
+      <c r="I97" s="2">
+        <f t="shared" si="7"/>
+        <v>91</v>
+      </c>
+      <c r="J97" s="3">
+        <v>437.82787401765262</v>
+      </c>
+      <c r="K97" s="3">
+        <v>1294.7575411901171</v>
+      </c>
+    </row>
+    <row r="98" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D98" s="2">
+        <f t="shared" si="6"/>
+        <v>92</v>
+      </c>
+      <c r="E98" s="3">
+        <v>462.35614917610269</v>
+      </c>
+      <c r="F98" s="3">
+        <v>1239.083929458199</v>
+      </c>
+      <c r="I98" s="2">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+      <c r="J98" s="3">
+        <v>451.31409343465009</v>
+      </c>
+      <c r="K98" s="3">
+        <v>1209.073579509391</v>
+      </c>
+    </row>
+    <row r="99" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D99" s="2">
+        <f t="shared" si="6"/>
+        <v>93</v>
+      </c>
+      <c r="E99" s="3">
+        <v>469.29687548665453</v>
+      </c>
+      <c r="F99" s="3">
+        <v>1277.197314179371</v>
+      </c>
+      <c r="I99" s="2">
+        <f t="shared" si="7"/>
+        <v>93</v>
+      </c>
+      <c r="J99" s="3">
+        <v>443.6216109207279</v>
+      </c>
+      <c r="K99" s="3">
+        <v>1214.30361213318</v>
+      </c>
+    </row>
+    <row r="100" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D100" s="2">
+        <f t="shared" si="6"/>
+        <v>94</v>
+      </c>
+      <c r="E100" s="3">
+        <v>474.79165153215558</v>
+      </c>
+      <c r="F100" s="3">
+        <v>1180.005950570642</v>
+      </c>
+      <c r="I100" s="2">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="J100" s="3">
+        <v>448.90605704733389</v>
+      </c>
+      <c r="K100" s="3">
+        <v>1413.372322216763</v>
+      </c>
+    </row>
+    <row r="101" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D101" s="2">
+        <f t="shared" si="6"/>
+        <v>95</v>
+      </c>
+      <c r="E101" s="3">
+        <v>467.74116803768231</v>
+      </c>
+      <c r="F101" s="3">
+        <v>1182.228168696483</v>
+      </c>
+      <c r="I101" s="2">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="J101" s="3">
+        <v>446.97385428023892</v>
+      </c>
+      <c r="K101" s="3">
+        <v>1360.579784747436</v>
+      </c>
+    </row>
+    <row r="102" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D102" s="2">
+        <f t="shared" si="6"/>
+        <v>96</v>
+      </c>
+      <c r="E102" s="3">
+        <v>471.19410489190477</v>
+      </c>
+      <c r="F102" s="3">
+        <v>1191.526198155168</v>
+      </c>
+      <c r="I102" s="2">
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+      <c r="J102" s="3">
+        <v>429.82298606201391</v>
+      </c>
+      <c r="K102" s="3">
+        <v>1336.9728470791799</v>
+      </c>
+    </row>
+    <row r="103" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D103" s="2">
+        <f t="shared" si="6"/>
+        <v>97</v>
+      </c>
+      <c r="E103" s="3">
+        <v>460.20906116444729</v>
+      </c>
+      <c r="F103" s="3">
+        <v>1322.6211378929629</v>
+      </c>
+      <c r="I103" s="2">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="J103" s="3">
+        <v>440.54967103929903</v>
+      </c>
+      <c r="K103" s="3">
+        <v>1240.764538232941</v>
+      </c>
+    </row>
+    <row r="104" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D104" s="2">
+        <f t="shared" si="6"/>
+        <v>98</v>
+      </c>
+      <c r="E104" s="3">
+        <v>474.25239221408663</v>
+      </c>
+      <c r="F104" s="3">
+        <v>1217.035875230725</v>
+      </c>
+      <c r="I104" s="2">
+        <f t="shared" si="7"/>
+        <v>98</v>
+      </c>
+      <c r="J104" s="3">
+        <v>452.94770433225892</v>
+      </c>
+      <c r="K104" s="3">
+        <v>1251.6176966607729</v>
+      </c>
+    </row>
+    <row r="105" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D105" s="2">
+        <f t="shared" si="6"/>
+        <v>99</v>
+      </c>
+      <c r="E105" s="3">
+        <v>471.22637457739751</v>
+      </c>
+      <c r="F105" s="3">
+        <v>1170.5462642903869</v>
+      </c>
+      <c r="I105" s="2">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="J105" s="3">
+        <v>450.54541745023749</v>
+      </c>
+      <c r="K105" s="3">
+        <v>1152.8254531642519</v>
+      </c>
+    </row>
+    <row r="106" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D106" s="2">
+        <f t="shared" si="6"/>
+        <v>100</v>
+      </c>
+      <c r="E106" s="3">
+        <v>445.06753435028128</v>
+      </c>
+      <c r="F106" s="3">
+        <v>1321.260007836762</v>
+      </c>
+      <c r="I106" s="2">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="J106" s="3">
+        <v>452.14836879219098</v>
+      </c>
+      <c r="K106" s="3">
+        <v>1184.335580443236</v>
+      </c>
+    </row>
+    <row r="110" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E110" s="3">
+        <f>AVERAGE(E7:E106)</f>
+        <v>466.22261802459047</v>
+      </c>
+      <c r="F110" s="3">
+        <f>AVERAGE(F7:F106)</f>
+        <v>1241.9820294451281</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J110" s="3">
+        <f>AVERAGE(J7:J106)</f>
+        <v>448.16042155127462</v>
+      </c>
+      <c r="K110" s="3">
+        <f>AVERAGE(K7:K106)</f>
+        <v>1234.9365746245157</v>
+      </c>
+    </row>
+    <row r="111" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E111" s="3">
+        <f>_xlfn.STDEV.S(E7:E106)</f>
+        <v>9.460060108464635</v>
+      </c>
+      <c r="F111" s="3">
+        <f>_xlfn.STDEV.S(F7:F106)</f>
+        <v>81.031046807146609</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J111" s="3">
+        <f>_xlfn.STDEV.S(J7:J106)</f>
+        <v>9.1320468828918795</v>
+      </c>
+      <c r="K111" s="3">
+        <f>_xlfn.STDEV.S(K7:K106)</f>
+        <v>84.785546101682783</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>